<commit_message>
Added spreadsheet for dark stress racemosa and wrightii
</commit_message>
<xml_diff>
--- a/methods/HPLC_standards.xlsx
+++ b/methods/HPLC_standards.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23530"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bca08_000\Documents\scutellariaMetabolites\methods\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Bryce\Research\scutellariaMetabolites\methods\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AA01C79-5F53-43CD-9BB2-C98F11E2CDEA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA5E1439-E332-46D9-A985-7CF35A3E3C3E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{75B3777B-BA7A-4C98-B4D5-CAF9E967F79D}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{75B3777B-BA7A-4C98-B4D5-CAF9E967F79D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
   <si>
     <t>chemical</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>100 ppm mix to add (microL)</t>
+  </si>
+  <si>
+    <t>scutellarin only</t>
+  </si>
+  <si>
+    <t>to make 100 ppm mix (uL)</t>
   </si>
 </sst>
 </file>
@@ -474,10 +480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{276B4C21-22EC-4D1A-87D8-0CC5B274EE7C}">
-  <dimension ref="A1:L29"/>
+  <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -983,6 +989,55 @@
         <v>500</v>
       </c>
     </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>14</v>
+      </c>
+      <c r="D33">
+        <v>4000</v>
+      </c>
+      <c r="E33">
+        <v>1.5</v>
+      </c>
+      <c r="F33">
+        <f>$E33*(100*0.001)/($D33*0.001)*1000</f>
+        <v>37.500000000000007</v>
+      </c>
+    </row>
+    <row r="34" spans="3:6" x14ac:dyDescent="0.25">
+      <c r="E34" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="F34">
+        <f>(E33*1000)-SUM(F33)</f>
+        <v>1462.5</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D16">
     <sortCondition ref="B2:B16"/>
@@ -991,5 +1046,6 @@
     <mergeCell ref="A21:D21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>